<commit_message>
adding R squared values
</commit_message>
<xml_diff>
--- a/subgraphs/all/corr_mcrae_cc.xlsx
+++ b/subgraphs/all/corr_mcrae_cc.xlsx
@@ -1700,6 +1700,20 @@
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.192754953558266"/>
+                  <c:y val="0.0726664791901012"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>corr_mcrae_cc.txt!$B$2:$B$516</c:f>
@@ -4818,11 +4832,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2097956440"/>
-        <c:axId val="2097749592"/>
+        <c:axId val="2082893496"/>
+        <c:axId val="2082975240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2097956440"/>
+        <c:axId val="2082893496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4851,12 +4865,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097749592"/>
+        <c:crossAx val="2082975240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2097749592"/>
+        <c:axId val="2082975240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4867,13 +4881,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097956440"/>
+        <c:crossAx val="2082893496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -4966,6 +4984,20 @@
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.176832435419257"/>
+                  <c:y val="0.23046706118257"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>corr_mcrae_cc.txt!$B$2:$B$516</c:f>
@@ -8084,11 +8116,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2097776936"/>
-        <c:axId val="2097993960"/>
+        <c:axId val="2084241224"/>
+        <c:axId val="2084244168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2097776936"/>
+        <c:axId val="2084241224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8117,12 +8149,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097993960"/>
+        <c:crossAx val="2084244168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2097993960"/>
+        <c:axId val="2084244168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8133,13 +8165,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097776936"/>
+        <c:crossAx val="2084241224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -8235,6 +8271,20 @@
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.188541013683969"/>
+                  <c:y val="0.163065719726211"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>corr_mcrae_cc.txt!$B$2:$B$516</c:f>
@@ -11353,11 +11403,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2099891512"/>
-        <c:axId val="2080205832"/>
+        <c:axId val="2084224296"/>
+        <c:axId val="2084320600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2099891512"/>
+        <c:axId val="2084224296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11367,12 +11417,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080205832"/>
+        <c:crossAx val="2084320600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2080205832"/>
+        <c:axId val="2084320600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11383,13 +11433,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099891512"/>
+        <c:crossAx val="2084224296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -11487,6 +11541,20 @@
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.181142312202791"/>
+                  <c:y val="0.389505929814329"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>corr_mcrae_cc.txt!$B$2:$B$516</c:f>
@@ -14605,11 +14673,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2100143192"/>
-        <c:axId val="2100077352"/>
+        <c:axId val="2082344792"/>
+        <c:axId val="2037775112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2100143192"/>
+        <c:axId val="2082344792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14638,12 +14706,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100077352"/>
+        <c:crossAx val="2037775112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2100077352"/>
+        <c:axId val="2037775112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14654,13 +14722,21 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100143192"/>
+        <c:crossAx val="2082344792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -15126,7 +15202,7 @@
   <dimension ref="A1:F516"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>